<commit_message>
updated fragility curve plot size
</commit_message>
<xml_diff>
--- a/examples/puerto_rico_stoch/data/data_W.xlsx
+++ b/examples/puerto_rico_stoch/data/data_W.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="217">
   <si>
     <t>connection</t>
   </si>
@@ -6565,7 +6565,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6660,15 +6660,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2041</v>
-      </c>
-      <c r="B8" s="3">
-        <v>65.41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>88</v>
-      </c>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Starting to update capacity analysis - updated
</commit_message>
<xml_diff>
--- a/examples/puerto_rico_stoch/data/data_W.xlsx
+++ b/examples/puerto_rico_stoch/data/data_W.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="221">
   <si>
     <t>connection</t>
   </si>
@@ -6858,7 +6858,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6953,7 +6953,15 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+      <c r="A8">
+        <v>2041</v>
+      </c>
+      <c r="B8" s="3">
+        <v>65.41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>